<commit_message>
updata bản cuối cho nhân viên
</commit_message>
<xml_diff>
--- a/excel_data/data_tt.xlsx
+++ b/excel_data/data_tt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\Desktop\Project\QLThueCaNhan\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6AB87A6-38B1-45AD-A498-58ED07B9151F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FD1E36-1C62-46C4-A669-8AC6928AF559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6429C15B-FDB4-4104-BE49-309683CB1D63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="111">
   <si>
     <t>ID_user</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Nhân viên</t>
   </si>
   <si>
-    <t>10,000,000</t>
-  </si>
-  <si>
     <t>hoang.thi.bich@techlearn.pka.vn</t>
   </si>
   <si>
@@ -80,9 +77,6 @@
     <t>Kế toán</t>
   </si>
   <si>
-    <t>20,000,000</t>
-  </si>
-  <si>
     <t>tran.van.an@techlearn.pka.vn</t>
   </si>
   <si>
@@ -92,81 +86,54 @@
     <t>Trưởng phòng</t>
   </si>
   <si>
-    <t>30,000,000</t>
-  </si>
-  <si>
     <t>pham.van.cuong@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Lê Thị Duyên</t>
   </si>
   <si>
-    <t>12,000,000</t>
-  </si>
-  <si>
     <t>le.thi.duyen@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Võ Văn Đức</t>
   </si>
   <si>
-    <t>22,000,000</t>
-  </si>
-  <si>
     <t>vo.van.duc@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Nguyễn Thị Hà</t>
   </si>
   <si>
-    <t>35,000,000</t>
-  </si>
-  <si>
     <t>nguyen.thi.ha@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Phạm Văn Hải</t>
   </si>
   <si>
-    <t>13,000,000</t>
-  </si>
-  <si>
     <t>pham.van.hai@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Lê Thị Hồng</t>
   </si>
   <si>
-    <t>21,500,000</t>
-  </si>
-  <si>
     <t>le.thi.hong@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Võ Văn Hùng</t>
   </si>
   <si>
-    <t>37,000,000</t>
-  </si>
-  <si>
     <t>vo.van.hung@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Trần Thị Minh</t>
   </si>
   <si>
-    <t>11,500,000</t>
-  </si>
-  <si>
     <t>tran.thi.minh@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Nguyễn Văn A</t>
   </si>
   <si>
-    <t>10,500,000</t>
-  </si>
-  <si>
     <t>nguyen.van.a@techlearn.pka.vn</t>
   </si>
   <si>
@@ -179,63 +146,42 @@
     <t>Phạm Văn C</t>
   </si>
   <si>
-    <t>40,000,000</t>
-  </si>
-  <si>
     <t>pham.van.c@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Trần Văn D</t>
   </si>
   <si>
-    <t>12,500,000</t>
-  </si>
-  <si>
     <t>tran.van.d@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Hoàng Thị E</t>
   </si>
   <si>
-    <t>21,000,000</t>
-  </si>
-  <si>
     <t>hoang.thi.e@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Nguyễn Văn F</t>
   </si>
   <si>
-    <t>38,000,000</t>
-  </si>
-  <si>
     <t>nguyen.van.f@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Lê Thị G</t>
   </si>
   <si>
-    <t>14,000,000</t>
-  </si>
-  <si>
     <t>le.thi.g@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Võ Văn H</t>
   </si>
   <si>
-    <t>23,000,000</t>
-  </si>
-  <si>
     <t>vo.van.h@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Phạm Văn I</t>
   </si>
   <si>
-    <t>39,000,000</t>
-  </si>
-  <si>
     <t>pham.van.i@techlearn.pka.vn</t>
   </si>
   <si>
@@ -248,36 +194,24 @@
     <t>Lê Văn K</t>
   </si>
   <si>
-    <t>13,500,000</t>
-  </si>
-  <si>
     <t>le.van.k@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Trần Thị L</t>
   </si>
   <si>
-    <t>24,000,000</t>
-  </si>
-  <si>
     <t>tran.thi.l@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Nguyễn Văn M</t>
   </si>
   <si>
-    <t>36,000,000</t>
-  </si>
-  <si>
     <t>nguyen.van.m@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Hoàng Thị N</t>
   </si>
   <si>
-    <t>11,800,000</t>
-  </si>
-  <si>
     <t>hoang.thi.n@techlearn.pka.vn</t>
   </si>
   <si>
@@ -290,36 +224,24 @@
     <t>Phạm Thị P</t>
   </si>
   <si>
-    <t>37,500,000</t>
-  </si>
-  <si>
     <t>pham.thi.p@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Lê Văn Q</t>
   </si>
   <si>
-    <t>12,300,000</t>
-  </si>
-  <si>
     <t>le.van.q@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Trần Thị R</t>
   </si>
   <si>
-    <t>22,800,000</t>
-  </si>
-  <si>
     <t>tran.thi.r@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Nguyễn Văn S</t>
   </si>
   <si>
-    <t>39,500,000</t>
-  </si>
-  <si>
     <t>nguyen.van.s@techlearn.pka.vn</t>
   </si>
   <si>
@@ -332,27 +254,18 @@
     <t>Lê Thị U</t>
   </si>
   <si>
-    <t>25,000,000</t>
-  </si>
-  <si>
     <t>le.thi.u@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Võ Văn V</t>
   </si>
   <si>
-    <t>34,000,000</t>
-  </si>
-  <si>
     <t>vo.van.v@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Trần Văn W</t>
   </si>
   <si>
-    <t>12,700,000</t>
-  </si>
-  <si>
     <t>tran.van.w@techlearn.pka.vn</t>
   </si>
   <si>
@@ -365,18 +278,12 @@
     <t>Nguyễn Thị Y</t>
   </si>
   <si>
-    <t>40,500,000</t>
-  </si>
-  <si>
     <t>nguyen.thi.y@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Lê Thị Z</t>
   </si>
   <si>
-    <t>14,500,000</t>
-  </si>
-  <si>
     <t>le.thi.z@techlearn.pka.vn</t>
   </si>
   <si>
@@ -389,27 +296,18 @@
     <t>Hoàng Văn BB</t>
   </si>
   <si>
-    <t>38,500,000</t>
-  </si>
-  <si>
     <t>hoang.van.bb@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Võ Thị CC</t>
   </si>
   <si>
-    <t>12,800,000</t>
-  </si>
-  <si>
     <t>vo.thi.cc@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Lê Văn DD</t>
   </si>
   <si>
-    <t>23,300,000</t>
-  </si>
-  <si>
     <t>le.van.dd@techlearn.pka.vn</t>
   </si>
   <si>
@@ -422,18 +320,12 @@
     <t>Nguyễn Thị FF</t>
   </si>
   <si>
-    <t>11,700,000</t>
-  </si>
-  <si>
     <t>nguyen.thi.ff@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Trần Văn GG</t>
   </si>
   <si>
-    <t>24,500,000</t>
-  </si>
-  <si>
     <t>tran.van.gg@techlearn.pka.vn</t>
   </si>
   <si>
@@ -446,18 +338,12 @@
     <t>Lê Văn II</t>
   </si>
   <si>
-    <t>13,200,000</t>
-  </si>
-  <si>
     <t>le.van.ii@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Phạm Thị JJ</t>
   </si>
   <si>
-    <t>22,700,000</t>
-  </si>
-  <si>
     <t>pham.thi.jj@techlearn.pka.vn</t>
   </si>
   <si>
@@ -470,16 +356,10 @@
     <t>Hoàng Văn LL</t>
   </si>
   <si>
-    <t>12,600,000</t>
-  </si>
-  <si>
     <t>hoang.van.ll@techlearn.pka.vn</t>
   </si>
   <si>
     <t>Võ Thị MM</t>
-  </si>
-  <si>
-    <t>23,800,000</t>
   </si>
   <si>
     <t>vo.thi.mm@techlearn.pka.vn</t>
@@ -549,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -559,6 +439,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -897,7 +792,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -905,8 +800,8 @@
     <col min="1" max="1" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" style="8" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="2" bestFit="1" customWidth="1"/>
@@ -923,10 +818,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -949,14 +844,14 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5">
+        <v>10000000</v>
+      </c>
+      <c r="E2" s="5">
+        <v>977381889</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" s="3">
-        <v>977381889</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -970,19 +865,19 @@
         <v>20212002</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="5">
+        <v>20000000</v>
+      </c>
+      <c r="E3" s="5">
+        <v>953341893</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3">
-        <v>953341893</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -996,19 +891,19 @@
         <v>20222003</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5">
+        <v>30000000</v>
+      </c>
+      <c r="E4" s="5">
+        <v>963939620</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3">
-        <v>963939620</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -1022,19 +917,19 @@
         <v>20232004</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="5">
+        <v>12000000</v>
+      </c>
+      <c r="E5" s="5">
         <v>935424672</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G5" s="3">
         <v>1</v>
@@ -1048,19 +943,19 @@
         <v>20202005</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="3">
+        <v>12</v>
+      </c>
+      <c r="D6" s="5">
+        <v>22000000</v>
+      </c>
+      <c r="E6" s="5">
         <v>928488864</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G6" s="3">
         <v>3</v>
@@ -1074,19 +969,19 @@
         <v>20212006</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="3">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5">
+        <v>35000000</v>
+      </c>
+      <c r="E7" s="5">
         <v>990175229</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G7" s="3">
         <v>2</v>
@@ -1100,19 +995,19 @@
         <v>20222007</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="3">
+      <c r="D8" s="5">
+        <v>13000000</v>
+      </c>
+      <c r="E8" s="5">
         <v>952505760</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1126,19 +1021,19 @@
         <v>20232008</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="3">
+        <v>12</v>
+      </c>
+      <c r="D9" s="5">
+        <v>21500000</v>
+      </c>
+      <c r="E9" s="5">
         <v>972898910</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="G9" s="3">
         <v>4</v>
@@ -1152,19 +1047,19 @@
         <v>20242009</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="3">
+        <v>15</v>
+      </c>
+      <c r="D10" s="5">
+        <v>37000000</v>
+      </c>
+      <c r="E10" s="5">
         <v>957540008</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G10" s="3">
         <v>2</v>
@@ -1178,19 +1073,19 @@
         <v>20202010</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E11" s="3">
+      <c r="D11" s="5">
+        <v>11500000</v>
+      </c>
+      <c r="E11" s="5">
         <v>973378673</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3">
         <v>1</v>
@@ -1204,19 +1099,19 @@
         <v>20202011</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="3">
+      <c r="D12" s="5">
+        <v>10500000</v>
+      </c>
+      <c r="E12" s="5">
         <v>912345678</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3">
         <v>2</v>
@@ -1230,19 +1125,19 @@
         <v>20212012</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="3">
+        <v>12</v>
+      </c>
+      <c r="D13" s="5">
+        <v>22000000</v>
+      </c>
+      <c r="E13" s="5">
         <v>987654321</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -1256,19 +1151,19 @@
         <v>20222013</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="3">
+        <v>15</v>
+      </c>
+      <c r="D14" s="5">
+        <v>40000000</v>
+      </c>
+      <c r="E14" s="5">
         <v>978123456</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G14" s="3">
         <v>3</v>
@@ -1282,19 +1177,19 @@
         <v>20232014</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E15" s="3">
+      <c r="D15" s="5">
+        <v>12500000</v>
+      </c>
+      <c r="E15" s="5">
         <v>967543210</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G15" s="3">
         <v>1</v>
@@ -1308,19 +1203,19 @@
         <v>20202015</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E16" s="3">
+        <v>12</v>
+      </c>
+      <c r="D16" s="5">
+        <v>21000000</v>
+      </c>
+      <c r="E16" s="5">
         <v>930123456</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G16" s="3">
         <v>2</v>
@@ -1334,19 +1229,19 @@
         <v>20212016</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E17" s="3">
+        <v>15</v>
+      </c>
+      <c r="D17" s="5">
+        <v>38000000</v>
+      </c>
+      <c r="E17" s="5">
         <v>901234567</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G17" s="3">
         <v>0</v>
@@ -1360,19 +1255,19 @@
         <v>20222017</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="D18" s="5">
+        <v>14000000</v>
+      </c>
+      <c r="E18" s="5">
         <v>923456789</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="G18" s="3">
         <v>3</v>
@@ -1386,19 +1281,19 @@
         <v>20232018</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="3">
+        <v>12</v>
+      </c>
+      <c r="D19" s="5">
+        <v>23000000</v>
+      </c>
+      <c r="E19" s="5">
         <v>918123456</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="G19" s="3">
         <v>1</v>
@@ -1412,19 +1307,19 @@
         <v>20242019</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" s="3">
+        <v>15</v>
+      </c>
+      <c r="D20" s="5">
+        <v>39000000</v>
+      </c>
+      <c r="E20" s="5">
         <v>936543210</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="G20" s="3">
         <v>2</v>
@@ -1438,19 +1333,19 @@
         <v>20202020</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="3">
+      <c r="D21" s="5">
+        <v>12000000</v>
+      </c>
+      <c r="E21" s="5">
         <v>973456789</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="G21" s="3">
         <v>1</v>
@@ -1464,19 +1359,19 @@
         <v>20202021</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="3">
+      <c r="D22" s="5">
+        <v>13500000</v>
+      </c>
+      <c r="E22" s="5">
         <v>974567890</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="G22" s="3">
         <v>0</v>
@@ -1490,19 +1385,19 @@
         <v>20212022</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="3">
+        <v>12</v>
+      </c>
+      <c r="D23" s="5">
+        <v>24000000</v>
+      </c>
+      <c r="E23" s="5">
         <v>983456781</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="G23" s="3">
         <v>2</v>
@@ -1516,19 +1411,19 @@
         <v>20222023</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E24" s="3">
+        <v>15</v>
+      </c>
+      <c r="D24" s="5">
+        <v>36000000</v>
+      </c>
+      <c r="E24" s="5">
         <v>961239874</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="G24" s="3">
         <v>1</v>
@@ -1542,19 +1437,19 @@
         <v>20232024</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="3">
+      <c r="D25" s="5">
+        <v>11800000</v>
+      </c>
+      <c r="E25" s="5">
         <v>937654320</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="G25" s="3">
         <v>1</v>
@@ -1568,19 +1463,19 @@
         <v>20202025</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="3">
+        <v>12</v>
+      </c>
+      <c r="D26" s="5">
+        <v>23000000</v>
+      </c>
+      <c r="E26" s="5">
         <v>929876543</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="G26" s="3">
         <v>3</v>
@@ -1594,19 +1489,19 @@
         <v>20212026</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E27" s="3">
+        <v>15</v>
+      </c>
+      <c r="D27" s="5">
+        <v>37500000</v>
+      </c>
+      <c r="E27" s="5">
         <v>953214567</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>85</v>
+        <v>62</v>
       </c>
       <c r="G27" s="3">
         <v>2</v>
@@ -1620,19 +1515,19 @@
         <v>20222027</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" s="3">
+      <c r="D28" s="5">
+        <v>12300000</v>
+      </c>
+      <c r="E28" s="5">
         <v>913456782</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="G28" s="3">
         <v>1</v>
@@ -1646,19 +1541,19 @@
         <v>20232028</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E29" s="3">
+        <v>12</v>
+      </c>
+      <c r="D29" s="5">
+        <v>22800000</v>
+      </c>
+      <c r="E29" s="5">
         <v>908765432</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="G29" s="3">
         <v>0</v>
@@ -1672,19 +1567,19 @@
         <v>20242029</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="3">
+        <v>15</v>
+      </c>
+      <c r="D30" s="5">
+        <v>39500000</v>
+      </c>
+      <c r="E30" s="5">
         <v>976548901</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="G30" s="3">
         <v>1</v>
@@ -1698,19 +1593,19 @@
         <v>20202030</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="3">
+      <c r="D31" s="5">
+        <v>13000000</v>
+      </c>
+      <c r="E31" s="5">
         <v>921234567</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="G31" s="3">
         <v>2</v>
@@ -1724,19 +1619,19 @@
         <v>20212031</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E32" s="3">
+        <v>12</v>
+      </c>
+      <c r="D32" s="5">
+        <v>25000000</v>
+      </c>
+      <c r="E32" s="5">
         <v>903459876</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="G32" s="3">
         <v>4</v>
@@ -1750,19 +1645,19 @@
         <v>20222032</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="E33" s="3">
+        <v>15</v>
+      </c>
+      <c r="D33" s="5">
+        <v>34000000</v>
+      </c>
+      <c r="E33" s="5">
         <v>934567890</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="G33" s="3">
         <v>3</v>
@@ -1776,19 +1671,19 @@
         <v>20232033</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>103</v>
+        <v>75</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="E34" s="3">
+      <c r="D34" s="5">
+        <v>12700000</v>
+      </c>
+      <c r="E34" s="5">
         <v>967891234</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="G34" s="3">
         <v>1</v>
@@ -1802,19 +1697,19 @@
         <v>20202034</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E35" s="3">
+        <v>12</v>
+      </c>
+      <c r="D35" s="5">
+        <v>21500000</v>
+      </c>
+      <c r="E35" s="5">
         <v>978123456</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>107</v>
+        <v>78</v>
       </c>
       <c r="G35" s="3">
         <v>0</v>
@@ -1828,19 +1723,19 @@
         <v>20212035</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E36" s="3">
+        <v>15</v>
+      </c>
+      <c r="D36" s="5">
+        <v>40500000</v>
+      </c>
+      <c r="E36" s="5">
         <v>958765432</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="G36" s="3">
         <v>2</v>
@@ -1854,19 +1749,19 @@
         <v>20222036</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E37" s="3">
+      <c r="D37" s="5">
+        <v>14500000</v>
+      </c>
+      <c r="E37" s="5">
         <v>903456782</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="G37" s="3">
         <v>3</v>
@@ -1880,19 +1775,19 @@
         <v>20232037</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E38" s="3">
+        <v>12</v>
+      </c>
+      <c r="D38" s="5">
+        <v>22000000</v>
+      </c>
+      <c r="E38" s="5">
         <v>912345678</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="G38" s="3">
         <v>1</v>
@@ -1906,19 +1801,19 @@
         <v>20242038</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="E39" s="3">
+        <v>15</v>
+      </c>
+      <c r="D39" s="5">
+        <v>38500000</v>
+      </c>
+      <c r="E39" s="5">
         <v>965432109</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
       <c r="G39" s="3">
         <v>2</v>
@@ -1932,19 +1827,19 @@
         <v>20202039</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>119</v>
+        <v>87</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E40" s="3">
+      <c r="D40" s="5">
+        <v>12800000</v>
+      </c>
+      <c r="E40" s="5">
         <v>956781234</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>121</v>
+        <v>88</v>
       </c>
       <c r="G40" s="3">
         <v>1</v>
@@ -1958,19 +1853,19 @@
         <v>20212040</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="3">
+        <v>12</v>
+      </c>
+      <c r="D41" s="5">
+        <v>23300000</v>
+      </c>
+      <c r="E41" s="5">
         <v>923456781</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>124</v>
+        <v>90</v>
       </c>
       <c r="G41" s="3">
         <v>4</v>
@@ -1984,19 +1879,19 @@
         <v>20222041</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>125</v>
+        <v>91</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E42" s="3">
+        <v>15</v>
+      </c>
+      <c r="D42" s="5">
+        <v>35000000</v>
+      </c>
+      <c r="E42" s="5">
         <v>938765432</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="G42" s="3">
         <v>0</v>
@@ -2010,19 +1905,19 @@
         <v>20232042</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E43" s="3">
+      <c r="D43" s="5">
+        <v>11700000</v>
+      </c>
+      <c r="E43" s="5">
         <v>973456781</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="G43" s="3">
         <v>2</v>
@@ -2036,19 +1931,19 @@
         <v>20202043</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" s="3">
+        <v>12</v>
+      </c>
+      <c r="D44" s="5">
+        <v>24500000</v>
+      </c>
+      <c r="E44" s="5">
         <v>908765432</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>132</v>
+        <v>96</v>
       </c>
       <c r="G44" s="3">
         <v>1</v>
@@ -2062,19 +1957,19 @@
         <v>20212044</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>133</v>
+        <v>97</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E45" s="3">
+        <v>15</v>
+      </c>
+      <c r="D45" s="5">
+        <v>37000000</v>
+      </c>
+      <c r="E45" s="5">
         <v>952345678</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="G45" s="3">
         <v>3</v>
@@ -2088,19 +1983,19 @@
         <v>20222045</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E46" s="3">
+      <c r="D46" s="5">
+        <v>13200000</v>
+      </c>
+      <c r="E46" s="5">
         <v>918765432</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="G46" s="3">
         <v>0</v>
@@ -2114,19 +2009,19 @@
         <v>20232046</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>138</v>
+        <v>101</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" s="3">
+        <v>12</v>
+      </c>
+      <c r="D47" s="5">
+        <v>22700000</v>
+      </c>
+      <c r="E47" s="5">
         <v>936543210</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="G47" s="3">
         <v>1</v>
@@ -2140,19 +2035,19 @@
         <v>20242047</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="3">
+        <v>15</v>
+      </c>
+      <c r="D48" s="5">
+        <v>39000000</v>
+      </c>
+      <c r="E48" s="5">
         <v>967654321</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="G48" s="3">
         <v>2</v>
@@ -2166,19 +2061,19 @@
         <v>20202048</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E49" s="3">
+      <c r="D49" s="5">
+        <v>12600000</v>
+      </c>
+      <c r="E49" s="5">
         <v>971234567</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>145</v>
+        <v>106</v>
       </c>
       <c r="G49" s="3">
         <v>1</v>
@@ -2192,19 +2087,19 @@
         <v>20212049</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="E50" s="3">
+        <v>12</v>
+      </c>
+      <c r="D50" s="5">
+        <v>23800000</v>
+      </c>
+      <c r="E50" s="5">
         <v>926543210</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>148</v>
+        <v>108</v>
       </c>
       <c r="G50" s="3">
         <v>3</v>
@@ -2218,19 +2113,19 @@
         <v>20222050</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E51" s="3">
+        <v>15</v>
+      </c>
+      <c r="D51" s="5">
+        <v>40000000</v>
+      </c>
+      <c r="E51" s="5">
         <v>951234567</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>150</v>
+        <v>110</v>
       </c>
       <c r="G51" s="3">
         <v>0</v>

</xml_diff>

<commit_message>
Add tax calculation guidelines and update employee tax display table
</commit_message>
<xml_diff>
--- a/excel_data/data_tt.xlsx
+++ b/excel_data/data_tt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\Desktop\Project\QLThueCaNhan\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC610D3C-B956-47AD-84C4-6C2D1B943EB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FABD2F6-A448-4BA5-ACBF-584A26A129F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6429C15B-FDB4-4104-BE49-309683CB1D63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="112">
   <si>
     <t>ID_user</t>
   </si>
@@ -165,6 +165,213 @@
   </si>
   <si>
     <t>nguyen.van.f@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Năm </t>
+  </si>
+  <si>
+    <t>Lê Thị G</t>
+  </si>
+  <si>
+    <t>le.thi.g@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Võ Văn H</t>
+  </si>
+  <si>
+    <t>vo.van.h@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Phạm Văn I</t>
+  </si>
+  <si>
+    <t>pham.van.i@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị J</t>
+  </si>
+  <si>
+    <t>nguyen.thi.j@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Lê Văn K</t>
+  </si>
+  <si>
+    <t>le.van.k@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Trần Thị L</t>
+  </si>
+  <si>
+    <t>tran.thi.l@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn M</t>
+  </si>
+  <si>
+    <t>nguyen.van.m@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Hoàng Thị N</t>
+  </si>
+  <si>
+    <t>hoang.thi.n@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Võ Văn O</t>
+  </si>
+  <si>
+    <t>vo.van.o@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Phạm Thị P</t>
+  </si>
+  <si>
+    <t>pham.thi.p@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Lê Văn Q</t>
+  </si>
+  <si>
+    <t>le.van.q@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Trần Thị R</t>
+  </si>
+  <si>
+    <t>tran.thi.r@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn S</t>
+  </si>
+  <si>
+    <t>nguyen.van.s@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Hoàng Văn T</t>
+  </si>
+  <si>
+    <t>hoang.van.t@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Lê Thị U</t>
+  </si>
+  <si>
+    <t>le.thi.u@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Võ Văn V</t>
+  </si>
+  <si>
+    <t>vo.van.v@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Trần Văn W</t>
+  </si>
+  <si>
+    <t>tran.van.w@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Phạm Văn X</t>
+  </si>
+  <si>
+    <t>pham.van.x@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị Y</t>
+  </si>
+  <si>
+    <t>nguyen.thi.y@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Lê Thị Z</t>
+  </si>
+  <si>
+    <t>le.thi.z@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Trần Văn AA</t>
+  </si>
+  <si>
+    <t>tran.van.aa@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Hoàng Văn BB</t>
+  </si>
+  <si>
+    <t>hoang.van.bb@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Võ Thị CC</t>
+  </si>
+  <si>
+    <t>vo.thi.cc@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Lê Văn DD</t>
+  </si>
+  <si>
+    <t>le.van.dd@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Phạm Văn EE</t>
+  </si>
+  <si>
+    <t>pham.van.ee@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị FF</t>
+  </si>
+  <si>
+    <t>nguyen.thi.ff@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Trần Văn GG</t>
+  </si>
+  <si>
+    <t>tran.van.gg@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Võ Thị HH</t>
+  </si>
+  <si>
+    <t>vo.thi.hh@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Lê Văn II</t>
+  </si>
+  <si>
+    <t>le.van.ii@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Phạm Thị JJ</t>
+  </si>
+  <si>
+    <t>pham.thi.jj@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn KK</t>
+  </si>
+  <si>
+    <t>nguyen.van.kk@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Hoàng Văn LL</t>
+  </si>
+  <si>
+    <t>hoang.van.ll@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Võ Thị MM</t>
+  </si>
+  <si>
+    <t>vo.thi.mm@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Lê Văn NN</t>
+  </si>
+  <si>
+    <t>le.van.nn@techlearn.pka.vn</t>
   </si>
 </sst>
 </file>
@@ -225,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -236,11 +443,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6313BFD-A3F9-4365-BB48-007C685AF90C}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,7 +795,7 @@
     <col min="1" max="1" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13" style="4" customWidth="1"/>
     <col min="5" max="5" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
@@ -595,7 +803,7 @@
     <col min="9" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -605,7 +813,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -620,8 +828,11 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>20202001</v>
       </c>
@@ -631,7 +842,7 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>10000000</v>
       </c>
       <c r="E2" s="3">
@@ -646,8 +857,11 @@
       <c r="H2" s="3">
         <v>1234</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I2" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>20212002</v>
       </c>
@@ -657,7 +871,7 @@
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>20000000</v>
       </c>
       <c r="E3" s="3">
@@ -672,8 +886,11 @@
       <c r="H3" s="3">
         <v>1234</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I3" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>20222003</v>
       </c>
@@ -683,7 +900,7 @@
       <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>30000000</v>
       </c>
       <c r="E4" s="3">
@@ -693,13 +910,16 @@
         <v>16</v>
       </c>
       <c r="G4" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3">
         <v>1234</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20232004</v>
       </c>
@@ -709,7 +929,7 @@
       <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>12000000</v>
       </c>
       <c r="E5" s="3">
@@ -724,8 +944,11 @@
       <c r="H5" s="3">
         <v>1122</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>20202005</v>
       </c>
@@ -735,7 +958,7 @@
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>22000000</v>
       </c>
       <c r="E6" s="3">
@@ -750,8 +973,11 @@
       <c r="H6" s="3">
         <v>3344</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>20212006</v>
       </c>
@@ -761,7 +987,7 @@
       <c r="C7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>35000000</v>
       </c>
       <c r="E7" s="3">
@@ -776,8 +1002,11 @@
       <c r="H7" s="3">
         <v>5566</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>20222007</v>
       </c>
@@ -787,7 +1016,7 @@
       <c r="C8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>13000000</v>
       </c>
       <c r="E8" s="3">
@@ -802,8 +1031,11 @@
       <c r="H8" s="3">
         <v>7788</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>20232008</v>
       </c>
@@ -813,7 +1045,7 @@
       <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>21500000</v>
       </c>
       <c r="E9" s="3">
@@ -828,8 +1060,11 @@
       <c r="H9" s="3">
         <v>9900</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>20242009</v>
       </c>
@@ -839,7 +1074,7 @@
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>37000000</v>
       </c>
       <c r="E10" s="3">
@@ -854,8 +1089,11 @@
       <c r="H10" s="3">
         <v>1212</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>20202010</v>
       </c>
@@ -865,7 +1103,7 @@
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="6">
         <v>11500000</v>
       </c>
       <c r="E11" s="3">
@@ -880,8 +1118,11 @@
       <c r="H11" s="3">
         <v>3434</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>20202011</v>
       </c>
@@ -891,7 +1132,7 @@
       <c r="C12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
         <v>10500000</v>
       </c>
       <c r="E12" s="3">
@@ -906,8 +1147,11 @@
       <c r="H12" s="3">
         <v>1235</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>20212012</v>
       </c>
@@ -917,7 +1161,7 @@
       <c r="C13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="6">
         <v>22000000</v>
       </c>
       <c r="E13" s="3">
@@ -932,8 +1176,11 @@
       <c r="H13" s="3">
         <v>5679</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>20222013</v>
       </c>
@@ -943,7 +1190,7 @@
       <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="6">
         <v>40000000</v>
       </c>
       <c r="E14" s="3">
@@ -958,8 +1205,11 @@
       <c r="H14" s="3">
         <v>9102</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>20232014</v>
       </c>
@@ -969,7 +1219,7 @@
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="6">
         <v>12500000</v>
       </c>
       <c r="E15" s="3">
@@ -984,8 +1234,11 @@
       <c r="H15" s="3">
         <v>1123</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I15" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>20202015</v>
       </c>
@@ -995,7 +1248,7 @@
       <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="6">
         <v>21000000</v>
       </c>
       <c r="E16" s="3">
@@ -1010,8 +1263,11 @@
       <c r="H16" s="3">
         <v>3345</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>20212016</v>
       </c>
@@ -1021,7 +1277,7 @@
       <c r="C17" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="6">
         <v>38000000</v>
       </c>
       <c r="E17" s="3">
@@ -1035,6 +1291,995 @@
       </c>
       <c r="H17" s="3">
         <v>5567</v>
+      </c>
+      <c r="I17" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>20222017</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="6">
+        <v>14000000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>923456789</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="3">
+        <v>3</v>
+      </c>
+      <c r="H18" s="3">
+        <v>7789</v>
+      </c>
+      <c r="I18" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>20232018</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="6">
+        <v>23000000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>918123456</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>9901</v>
+      </c>
+      <c r="I19" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>20242019</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="6">
+        <v>39000000</v>
+      </c>
+      <c r="E20" s="3">
+        <v>936543210</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="3">
+        <v>1213</v>
+      </c>
+      <c r="I20" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20202020</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="6">
+        <v>12000000</v>
+      </c>
+      <c r="E21" s="3">
+        <v>973456789</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1</v>
+      </c>
+      <c r="H21" s="3">
+        <v>3435</v>
+      </c>
+      <c r="I21" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>20202021</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="6">
+        <v>13500000</v>
+      </c>
+      <c r="E22" s="3">
+        <v>974567890</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1236</v>
+      </c>
+      <c r="I22" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>20212022</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" s="6">
+        <v>24000000</v>
+      </c>
+      <c r="E23" s="3">
+        <v>983456781</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G23" s="3">
+        <v>2</v>
+      </c>
+      <c r="H23" s="3">
+        <v>5670</v>
+      </c>
+      <c r="I23" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>20222023</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="6">
+        <v>36000000</v>
+      </c>
+      <c r="E24" s="3">
+        <v>961239874</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="3">
+        <v>1</v>
+      </c>
+      <c r="H24" s="3">
+        <v>9103</v>
+      </c>
+      <c r="I24" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>20232024</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="6">
+        <v>11800000</v>
+      </c>
+      <c r="E25" s="3">
+        <v>937654320</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
+      <c r="H25" s="3">
+        <v>1124</v>
+      </c>
+      <c r="I25" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>20202025</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="6">
+        <v>23000000</v>
+      </c>
+      <c r="E26" s="3">
+        <v>929876543</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G26" s="3">
+        <v>3</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3346</v>
+      </c>
+      <c r="I26" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>20212026</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="6">
+        <v>37500000</v>
+      </c>
+      <c r="E27" s="3">
+        <v>953214567</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="3">
+        <v>2</v>
+      </c>
+      <c r="H27" s="3">
+        <v>5568</v>
+      </c>
+      <c r="I27" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>20222027</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="6">
+        <v>12300000</v>
+      </c>
+      <c r="E28" s="3">
+        <v>913456782</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G28" s="3">
+        <v>1</v>
+      </c>
+      <c r="H28" s="3">
+        <v>7790</v>
+      </c>
+      <c r="I28" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>20232028</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="6">
+        <v>22800000</v>
+      </c>
+      <c r="E29" s="3">
+        <v>908765432</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0</v>
+      </c>
+      <c r="H29" s="3">
+        <v>9902</v>
+      </c>
+      <c r="I29" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>20242029</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="6">
+        <v>39500000</v>
+      </c>
+      <c r="E30" s="3">
+        <v>976548901</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
+      <c r="H30" s="3">
+        <v>1214</v>
+      </c>
+      <c r="I30" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>20202030</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="6">
+        <v>13000000</v>
+      </c>
+      <c r="E31" s="3">
+        <v>921234567</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G31" s="3">
+        <v>2</v>
+      </c>
+      <c r="H31" s="3">
+        <v>3436</v>
+      </c>
+      <c r="I31" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>20212031</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="6">
+        <v>25000000</v>
+      </c>
+      <c r="E32" s="3">
+        <v>903459876</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="3">
+        <v>4</v>
+      </c>
+      <c r="H32" s="3">
+        <v>5671</v>
+      </c>
+      <c r="I32" s="5">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>20222032</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="6">
+        <v>34000000</v>
+      </c>
+      <c r="E33" s="3">
+        <v>934567890</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" s="3">
+        <v>3</v>
+      </c>
+      <c r="H33" s="3">
+        <v>9104</v>
+      </c>
+      <c r="I33" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>20232033</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="6">
+        <v>12700000</v>
+      </c>
+      <c r="E34" s="3">
+        <v>967891234</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G34" s="3">
+        <v>1</v>
+      </c>
+      <c r="H34" s="3">
+        <v>1125</v>
+      </c>
+      <c r="I34" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>20202034</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="6">
+        <v>21500000</v>
+      </c>
+      <c r="E35" s="3">
+        <v>978123456</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" s="3">
+        <v>0</v>
+      </c>
+      <c r="H35" s="3">
+        <v>3347</v>
+      </c>
+      <c r="I35" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>20212035</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="6">
+        <v>40500000</v>
+      </c>
+      <c r="E36" s="3">
+        <v>958765432</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36" s="3">
+        <v>2</v>
+      </c>
+      <c r="H36" s="3">
+        <v>5569</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>20222036</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="6">
+        <v>14500000</v>
+      </c>
+      <c r="E37" s="3">
+        <v>903456782</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G37" s="3">
+        <v>3</v>
+      </c>
+      <c r="H37" s="3">
+        <v>7791</v>
+      </c>
+      <c r="I37" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>20232037</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" s="6">
+        <v>22000000</v>
+      </c>
+      <c r="E38" s="3">
+        <v>912345678</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1</v>
+      </c>
+      <c r="H38" s="3">
+        <v>9903</v>
+      </c>
+      <c r="I38" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>20242038</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="6">
+        <v>38500000</v>
+      </c>
+      <c r="E39" s="3">
+        <v>965432109</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" s="3">
+        <v>2</v>
+      </c>
+      <c r="H39" s="3">
+        <v>1215</v>
+      </c>
+      <c r="I39" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>20202039</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="6">
+        <v>12800000</v>
+      </c>
+      <c r="E40" s="3">
+        <v>956781234</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1</v>
+      </c>
+      <c r="H40" s="3">
+        <v>3437</v>
+      </c>
+      <c r="I40" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>20212040</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="6">
+        <v>23300000</v>
+      </c>
+      <c r="E41" s="3">
+        <v>923456781</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G41" s="3">
+        <v>4</v>
+      </c>
+      <c r="H41" s="3">
+        <v>5672</v>
+      </c>
+      <c r="I41" s="5">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>20222041</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="6">
+        <v>35000000</v>
+      </c>
+      <c r="E42" s="3">
+        <v>938765432</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="3">
+        <v>0</v>
+      </c>
+      <c r="H42" s="3">
+        <v>9105</v>
+      </c>
+      <c r="I42" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>20232042</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="6">
+        <v>11700000</v>
+      </c>
+      <c r="E43" s="3">
+        <v>973456781</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G43" s="3">
+        <v>2</v>
+      </c>
+      <c r="H43" s="3">
+        <v>1126</v>
+      </c>
+      <c r="I43" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>20202043</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" s="6">
+        <v>24500000</v>
+      </c>
+      <c r="E44" s="3">
+        <v>908765432</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1</v>
+      </c>
+      <c r="H44" s="3">
+        <v>3348</v>
+      </c>
+      <c r="I44" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>20212044</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="6">
+        <v>37000000</v>
+      </c>
+      <c r="E45" s="3">
+        <v>952345678</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G45" s="3">
+        <v>3</v>
+      </c>
+      <c r="H45" s="3">
+        <v>5570</v>
+      </c>
+      <c r="I45" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>20222045</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="6">
+        <v>13200000</v>
+      </c>
+      <c r="E46" s="3">
+        <v>918765432</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="G46" s="3">
+        <v>0</v>
+      </c>
+      <c r="H46" s="3">
+        <v>7792</v>
+      </c>
+      <c r="I46" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>20232046</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="6">
+        <v>22700000</v>
+      </c>
+      <c r="E47" s="3">
+        <v>936543210</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G47" s="3">
+        <v>1</v>
+      </c>
+      <c r="H47" s="3">
+        <v>9904</v>
+      </c>
+      <c r="I47" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>20242047</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="6">
+        <v>39000000</v>
+      </c>
+      <c r="E48" s="3">
+        <v>967654321</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G48" s="3">
+        <v>2</v>
+      </c>
+      <c r="H48" s="3">
+        <v>1216</v>
+      </c>
+      <c r="I48" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>20202048</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="6">
+        <v>12600000</v>
+      </c>
+      <c r="E49" s="3">
+        <v>971234567</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G49" s="3">
+        <v>1</v>
+      </c>
+      <c r="H49" s="3">
+        <v>3438</v>
+      </c>
+      <c r="I49" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" s="3">
+        <v>20212049</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="6">
+        <v>23800000</v>
+      </c>
+      <c r="E50" s="3">
+        <v>926543210</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G50" s="3">
+        <v>3</v>
+      </c>
+      <c r="H50" s="3">
+        <v>5673</v>
+      </c>
+      <c r="I50" s="5">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="3">
+        <v>20222050</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="6">
+        <v>40000000</v>
+      </c>
+      <c r="E51" s="3">
+        <v>951234567</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G51" s="3">
+        <v>0</v>
+      </c>
+      <c r="H51" s="3">
+        <v>9106</v>
+      </c>
+      <c r="I51" s="5">
+        <v>2024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor CSS for consistent layout and update HTML structure for employee management
</commit_message>
<xml_diff>
--- a/excel_data/data_tt.xlsx
+++ b/excel_data/data_tt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ThinkPad\Desktop\Project\QLThueCaNhan\excel_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FABD2F6-A448-4BA5-ACBF-584A26A129F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3FDE788-6A05-429A-AD8C-F5BFEA8E0946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6429C15B-FDB4-4104-BE49-309683CB1D63}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="119">
   <si>
     <t>ID_user</t>
   </si>
@@ -372,13 +372,34 @@
   </si>
   <si>
     <t>le.van.nn@techlearn.pka.vn</t>
+  </si>
+  <si>
+    <t>Phòng</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>Kinh doanh</t>
+  </si>
+  <si>
+    <t>Sale</t>
+  </si>
+  <si>
+    <t>Nhân sự</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Truyền thông</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,6 +415,14 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -432,7 +461,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -449,6 +478,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6313BFD-A3F9-4365-BB48-007C685AF90C}">
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D51"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -800,10 +835,13 @@
     <col min="6" max="6" width="30" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="8.88671875" style="2"/>
+    <col min="10" max="10" width="11.21875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -831,8 +869,12 @@
       <c r="I1" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>20202001</v>
       </c>
@@ -860,8 +902,12 @@
       <c r="I2" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K2" s="3"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>20212002</v>
       </c>
@@ -889,8 +935,12 @@
       <c r="I3" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>20222003</v>
       </c>
@@ -918,8 +968,12 @@
       <c r="I4" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K4" s="3"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>20232004</v>
       </c>
@@ -947,8 +1001,12 @@
       <c r="I5" s="5">
         <v>2021</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>20202005</v>
       </c>
@@ -976,8 +1034,12 @@
       <c r="I6" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>20212006</v>
       </c>
@@ -1005,8 +1067,12 @@
       <c r="I7" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>20222007</v>
       </c>
@@ -1034,8 +1100,12 @@
       <c r="I8" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K8" s="3"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>20232008</v>
       </c>
@@ -1063,8 +1133,12 @@
       <c r="I9" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>20242009</v>
       </c>
@@ -1092,8 +1166,12 @@
       <c r="I10" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>20202010</v>
       </c>
@@ -1121,8 +1199,12 @@
       <c r="I11" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>20202011</v>
       </c>
@@ -1150,8 +1232,12 @@
       <c r="I12" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>20212012</v>
       </c>
@@ -1179,8 +1265,12 @@
       <c r="I13" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>20222013</v>
       </c>
@@ -1188,10 +1278,10 @@
         <v>35</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D14" s="6">
-        <v>40000000</v>
+        <v>14000000</v>
       </c>
       <c r="E14" s="3">
         <v>978123456</v>
@@ -1208,8 +1298,12 @@
       <c r="I14" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>20232014</v>
       </c>
@@ -1237,8 +1331,12 @@
       <c r="I15" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>20202015</v>
       </c>
@@ -1246,10 +1344,10 @@
         <v>39</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D16" s="6">
-        <v>21000000</v>
+        <v>17000000</v>
       </c>
       <c r="E16" s="3">
         <v>930123456</v>
@@ -1266,8 +1364,12 @@
       <c r="I16" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>20212016</v>
       </c>
@@ -1275,10 +1377,10 @@
         <v>41</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D17" s="6">
-        <v>38000000</v>
+        <v>18000000</v>
       </c>
       <c r="E17" s="3">
         <v>901234567</v>
@@ -1295,8 +1397,12 @@
       <c r="I17" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>20222017</v>
       </c>
@@ -1324,8 +1430,12 @@
       <c r="I18" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>20232018</v>
       </c>
@@ -1333,10 +1443,10 @@
         <v>46</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D19" s="6">
-        <v>23000000</v>
+        <v>18000000</v>
       </c>
       <c r="E19" s="3">
         <v>918123456</v>
@@ -1353,8 +1463,12 @@
       <c r="I19" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J19" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>20242019</v>
       </c>
@@ -1362,10 +1476,10 @@
         <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D20" s="6">
-        <v>39000000</v>
+        <v>19000000</v>
       </c>
       <c r="E20" s="3">
         <v>936543210</v>
@@ -1382,8 +1496,12 @@
       <c r="I20" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J20" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>20202020</v>
       </c>
@@ -1411,8 +1529,12 @@
       <c r="I21" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>20202021</v>
       </c>
@@ -1440,8 +1562,12 @@
       <c r="I22" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J22" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>20212022</v>
       </c>
@@ -1449,10 +1575,10 @@
         <v>54</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D23" s="6">
-        <v>24000000</v>
+        <v>11000000</v>
       </c>
       <c r="E23" s="3">
         <v>983456781</v>
@@ -1469,8 +1595,12 @@
       <c r="I23" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J23" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>20222023</v>
       </c>
@@ -1478,10 +1608,10 @@
         <v>56</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D24" s="6">
-        <v>36000000</v>
+        <v>16000000</v>
       </c>
       <c r="E24" s="3">
         <v>961239874</v>
@@ -1498,8 +1628,12 @@
       <c r="I24" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J24" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>20232024</v>
       </c>
@@ -1527,8 +1661,12 @@
       <c r="I25" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>20202025</v>
       </c>
@@ -1536,10 +1674,10 @@
         <v>60</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D26" s="6">
-        <v>23000000</v>
+        <v>13000000</v>
       </c>
       <c r="E26" s="3">
         <v>929876543</v>
@@ -1556,8 +1694,12 @@
       <c r="I26" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>20212026</v>
       </c>
@@ -1565,10 +1707,10 @@
         <v>62</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D27" s="6">
-        <v>37500000</v>
+        <v>17500000</v>
       </c>
       <c r="E27" s="3">
         <v>953214567</v>
@@ -1585,8 +1727,12 @@
       <c r="I27" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J27" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>20222027</v>
       </c>
@@ -1614,8 +1760,12 @@
       <c r="I28" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J28" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>20232028</v>
       </c>
@@ -1623,10 +1773,10 @@
         <v>66</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D29" s="6">
-        <v>22800000</v>
+        <v>16800000</v>
       </c>
       <c r="E29" s="3">
         <v>908765432</v>
@@ -1643,8 +1793,12 @@
       <c r="I29" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J29" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>20242029</v>
       </c>
@@ -1652,10 +1806,10 @@
         <v>68</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D30" s="6">
-        <v>39500000</v>
+        <v>15000000</v>
       </c>
       <c r="E30" s="3">
         <v>976548901</v>
@@ -1672,8 +1826,12 @@
       <c r="I30" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J30" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>20202030</v>
       </c>
@@ -1701,8 +1859,12 @@
       <c r="I31" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J31" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>20212031</v>
       </c>
@@ -1710,10 +1872,10 @@
         <v>72</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D32" s="6">
-        <v>25000000</v>
+        <v>15000000</v>
       </c>
       <c r="E32" s="3">
         <v>903459876</v>
@@ -1730,8 +1892,12 @@
       <c r="I32" s="5">
         <v>2022</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J32" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>20222032</v>
       </c>
@@ -1739,10 +1905,10 @@
         <v>74</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D33" s="6">
-        <v>34000000</v>
+        <v>14000000</v>
       </c>
       <c r="E33" s="3">
         <v>934567890</v>
@@ -1759,8 +1925,12 @@
       <c r="I33" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J33" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K33" s="3"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>20232033</v>
       </c>
@@ -1788,8 +1958,12 @@
       <c r="I34" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J34" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>20202034</v>
       </c>
@@ -1817,8 +1991,12 @@
       <c r="I35" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K35" s="3"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>20212035</v>
       </c>
@@ -1846,8 +2024,12 @@
       <c r="I36" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J36" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>20222036</v>
       </c>
@@ -1875,8 +2057,12 @@
       <c r="I37" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J37" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="K37" s="3"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>20232037</v>
       </c>
@@ -1904,8 +2090,12 @@
       <c r="I38" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J38" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>20242038</v>
       </c>
@@ -1933,8 +2123,12 @@
       <c r="I39" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J39" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K39" s="3"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>20202039</v>
       </c>
@@ -1962,8 +2156,12 @@
       <c r="I40" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J40" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>20212040</v>
       </c>
@@ -1991,8 +2189,12 @@
       <c r="I41" s="5">
         <v>2023</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>20222041</v>
       </c>
@@ -2020,8 +2222,12 @@
       <c r="I42" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J42" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>20232042</v>
       </c>
@@ -2049,8 +2255,12 @@
       <c r="I43" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J43" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>20202043</v>
       </c>
@@ -2078,8 +2288,12 @@
       <c r="I44" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J44" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>20212044</v>
       </c>
@@ -2087,10 +2301,10 @@
         <v>98</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D45" s="6">
-        <v>37000000</v>
+        <v>17000000</v>
       </c>
       <c r="E45" s="3">
         <v>952345678</v>
@@ -2107,8 +2321,12 @@
       <c r="I45" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J45" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>20222045</v>
       </c>
@@ -2136,8 +2354,12 @@
       <c r="I46" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J46" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>20232046</v>
       </c>
@@ -2165,8 +2387,12 @@
       <c r="I47" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K47" s="3"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>20242047</v>
       </c>
@@ -2174,10 +2400,10 @@
         <v>104</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D48" s="6">
-        <v>39000000</v>
+        <v>19000000</v>
       </c>
       <c r="E48" s="3">
         <v>967654321</v>
@@ -2194,8 +2420,12 @@
       <c r="I48" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K48" s="3"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>20202048</v>
       </c>
@@ -2223,8 +2453,12 @@
       <c r="I49" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K49" s="3"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>20212049</v>
       </c>
@@ -2252,8 +2486,12 @@
       <c r="I50" s="5">
         <v>2024</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J50" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K50" s="3"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>20222050</v>
       </c>
@@ -2261,10 +2499,10 @@
         <v>110</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D51" s="6">
-        <v>40000000</v>
+        <v>17000000</v>
       </c>
       <c r="E51" s="3">
         <v>951234567</v>
@@ -2281,6 +2519,10 @@
       <c r="I51" s="5">
         <v>2024</v>
       </c>
+      <c r="J51" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="K51" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>